<commit_message>
generated copilot script test
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utiglobal-my.sharepoint.com/personal/ascinta_utiglobal_com/Documents/Documents/Excel Processor/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048A0711B51985ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{084D86B0-2681-4335-9F0B-70F8810E0855}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC1048A0711B51985ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C80E72A7-8B6C-496A-AEC5-DF029BEC2B11}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="7035" windowWidth="16410" windowHeight="14145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="2460" windowWidth="16410" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Types" sheetId="1" r:id="rId1"/>
@@ -26,50 +26,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Device Type Names</t>
-  </si>
-  <si>
-    <t>Device Abriviation</t>
-  </si>
-  <si>
-    <t>Associated Tests</t>
-  </si>
-  <si>
-    <t>Camera</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>CAM</t>
   </si>
   <si>
-    <t>Test_1, Test_2, Test_3, Test_4</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
     <t>INP</t>
   </si>
   <si>
-    <t>Test_1, Test_2, Test_4</t>
-  </si>
-  <si>
-    <t>Keypad</t>
-  </si>
-  <si>
     <t>KEY</t>
   </si>
   <si>
-    <t>Test_1, Test_3, Test_4</t>
-  </si>
-  <si>
     <t>GSS</t>
   </si>
   <si>
-    <t>Test_1, Test_2, Test_3</t>
-  </si>
-  <si>
     <t>Test_4</t>
   </si>
   <si>
@@ -82,7 +52,40 @@
     <t>Test_1</t>
   </si>
   <si>
-    <t>Test Types</t>
+    <t>Device Type</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Alt Text</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Test_1,Test_2,Test_3,Test_4</t>
+  </si>
+  <si>
+    <t>Test_1,Test_2,Test_4</t>
+  </si>
+  <si>
+    <t>Test_1,Test_3,Test_4</t>
+  </si>
+  <si>
+    <t>Test_1,Test_2,Test_3</t>
   </si>
 </sst>
 </file>
@@ -135,6 +138,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,72 +407,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -475,10 +466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6C1980-787E-45A4-9C26-FEAFB8033CB6}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,29 +477,44 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>